<commit_message>
Graphs for MAP added
</commit_message>
<xml_diff>
--- a/Results/OkapiBM-25.xlsx
+++ b/Results/OkapiBM-25.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="alpha" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="11">
   <si>
     <t>Beta</t>
   </si>
@@ -390,15 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L36"/>
+  <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -406,7 +406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -414,7 +414,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -422,7 +422,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -430,7 +430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -438,7 +438,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -446,12 +446,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -463,127 +463,439 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0.1</v>
       </c>
       <c r="C12">
-        <v>0.36280763416477702</v>
+        <f>AVERAGE(F$13:F$22)</f>
+        <v>0.36280763416477652</v>
       </c>
       <c r="D12">
         <f>AVERAGE(C$27:C$36)</f>
         <v>0.5099999999999999</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0.2</v>
       </c>
       <c r="C13">
-        <v>0.38087641723356003</v>
+        <f>AVERAGE(G$13:G$22)</f>
+        <v>0.36322430083144319</v>
       </c>
       <c r="D13">
         <f>AVERAGE(D$27:D$36)</f>
         <v>0.48</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="G13">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="H13">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="I13">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="J13">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="K13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="L13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="M13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="N13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="O13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.3</v>
       </c>
       <c r="C14">
-        <v>0.42021239606953797</v>
+        <f>AVERAGE(H$13:H$22)</f>
+        <v>0.41589361300075556</v>
       </c>
       <c r="D14">
         <f>AVERAGE(E$27:E$36)</f>
         <v>0.5099999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>0.18979591836734599</v>
+      </c>
+      <c r="G14">
+        <v>0.261224489795918</v>
+      </c>
+      <c r="H14">
+        <v>0.261224489795918</v>
+      </c>
+      <c r="I14">
+        <v>0.261224489795918</v>
+      </c>
+      <c r="J14">
+        <v>0.261224489795918</v>
+      </c>
+      <c r="K14">
+        <v>0.25170068027210801</v>
+      </c>
+      <c r="L14">
+        <v>0.25170068027210801</v>
+      </c>
+      <c r="M14">
+        <v>0.34693877551020402</v>
+      </c>
+      <c r="N14">
+        <v>0.37074829931972703</v>
+      </c>
+      <c r="O14">
+        <v>0.29931972789115602</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>0.4</v>
       </c>
       <c r="C15">
-        <v>0.45531887755102002</v>
+        <f>AVERAGE(I$13:I$22)</f>
+        <v>0.45531887755102024</v>
       </c>
       <c r="D15">
         <f>AVERAGE(F$27:F$36)</f>
         <v>0.48999999999999994</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="G15">
+        <v>0.6</v>
+      </c>
+      <c r="H15">
+        <v>0.6</v>
+      </c>
+      <c r="I15">
+        <v>0.6</v>
+      </c>
+      <c r="J15">
+        <v>0.37777777777777699</v>
+      </c>
+      <c r="K15">
+        <v>0.40277777777777701</v>
+      </c>
+      <c r="L15">
+        <v>0.40277777777777701</v>
+      </c>
+      <c r="M15">
+        <v>0.42063492063491997</v>
+      </c>
+      <c r="N15">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="O15">
+        <v>0.47777777777777702</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.5</v>
       </c>
       <c r="C16">
-        <v>0.43205168178382403</v>
+        <f>AVERAGE(J$13:J$22)</f>
+        <v>0.42313633786848043</v>
       </c>
       <c r="D16">
         <f>AVERAGE(G$27:G$36)</f>
         <v>0.51</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
+      </c>
+      <c r="K16">
+        <v>0.5</v>
+      </c>
+      <c r="L16">
+        <v>0.5</v>
+      </c>
+      <c r="M16">
+        <v>0.5</v>
+      </c>
+      <c r="N16">
+        <v>0.5</v>
+      </c>
+      <c r="O16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.6</v>
       </c>
       <c r="C17">
-        <v>0.42307350718065001</v>
+        <f>AVERAGE(K$13:K$22)</f>
+        <v>0.42307350718064962</v>
       </c>
       <c r="D17">
         <f>AVERAGE(H$27:H$36)</f>
         <v>0.52999999999999992</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>0.50925925925925897</v>
+      </c>
+      <c r="G17">
+        <v>0.47718253968253899</v>
+      </c>
+      <c r="H17">
+        <v>0.47718253968253899</v>
+      </c>
+      <c r="I17">
+        <v>0.56051587301587302</v>
+      </c>
+      <c r="J17">
+        <v>0.56051587301587302</v>
+      </c>
+      <c r="K17">
+        <v>0.47718253968253899</v>
+      </c>
+      <c r="L17">
+        <v>0.58068783068783003</v>
+      </c>
+      <c r="M17">
+        <v>0.44179894179894103</v>
+      </c>
+      <c r="N17">
+        <v>0.44179894179894103</v>
+      </c>
+      <c r="O17">
+        <v>0.469907407407407</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0.7</v>
       </c>
       <c r="C18">
-        <v>0.44382527084908002</v>
+        <f>AVERAGE(L$13:L$22)</f>
+        <v>0.44382527084907997</v>
       </c>
       <c r="D18">
         <f>AVERAGE(I$27:I$36)</f>
         <v>0.51</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0.45333333333333298</v>
+      </c>
+      <c r="G18">
+        <v>0.45333333333333298</v>
+      </c>
+      <c r="H18">
+        <v>0.6</v>
+      </c>
+      <c r="I18">
+        <v>0.4</v>
+      </c>
+      <c r="J18">
+        <v>0.4</v>
+      </c>
+      <c r="K18">
+        <v>0.6</v>
+      </c>
+      <c r="L18">
+        <v>0.6</v>
+      </c>
+      <c r="M18">
+        <v>0.65</v>
+      </c>
+      <c r="N18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="O18">
+        <v>0.63888888888888895</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0.79999999999999905</v>
       </c>
       <c r="C19">
-        <v>0.45887377173091398</v>
+        <f>AVERAGE(M$13:M$22)</f>
+        <v>0.45649281934996183</v>
       </c>
       <c r="D19">
         <f>AVERAGE(J$27:J$36)</f>
         <v>0.52999999999999992</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>0.36296296296296199</v>
+      </c>
+      <c r="G19">
+        <v>0.36296296296296199</v>
+      </c>
+      <c r="H19">
+        <v>0.36296296296296199</v>
+      </c>
+      <c r="I19">
+        <v>0.466269841269841</v>
+      </c>
+      <c r="J19">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K19">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="L19">
+        <v>0.438271604938271</v>
+      </c>
+      <c r="M19">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="N19">
+        <v>0.422222222222222</v>
+      </c>
+      <c r="O19">
+        <v>0.47777777777777702</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.89999999999999902</v>
       </c>
       <c r="C20">
-        <v>0.47031557067271301</v>
+        <f>AVERAGE(N$13:N$22)</f>
+        <v>0.47031557067271307</v>
       </c>
       <c r="D20">
         <f>AVERAGE(K$27:K$36)</f>
         <v>0.54999999999999993</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>0.52</v>
+      </c>
+      <c r="G20">
+        <v>0.52</v>
+      </c>
+      <c r="H20">
+        <v>0.52</v>
+      </c>
+      <c r="I20">
+        <v>0.7</v>
+      </c>
+      <c r="J20">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="K20">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="L20">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="M20">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="N20">
+        <v>0.73333333333333295</v>
+      </c>
+      <c r="O20">
+        <v>0.71428571428571397</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.999999999999999</v>
       </c>
       <c r="C21">
-        <v>0.48049193751574698</v>
+        <f>AVERAGE(O$13:O$22)</f>
+        <v>0.4804919375157467</v>
       </c>
       <c r="D21">
         <f>AVERAGE(L$27:L$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>0.43293650793650701</v>
+      </c>
+      <c r="G21">
+        <v>0.43293650793650701</v>
+      </c>
+      <c r="H21">
+        <v>0.39219576719576699</v>
+      </c>
+      <c r="I21">
+        <v>0.51825396825396797</v>
+      </c>
+      <c r="J21">
+        <v>0.51825396825396797</v>
+      </c>
+      <c r="K21">
+        <v>0.46111111111111103</v>
+      </c>
+      <c r="L21">
+        <v>0.468518518518518</v>
+      </c>
+      <c r="M21">
+        <v>0.468518518518518</v>
+      </c>
+      <c r="N21">
+        <v>0.64246031746031695</v>
+      </c>
+      <c r="O21">
+        <v>0.63165784832451399</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>0.207936507936507</v>
+      </c>
+      <c r="G22">
+        <v>0.207936507936507</v>
+      </c>
+      <c r="H22">
+        <v>0.212037037037037</v>
+      </c>
+      <c r="I22">
+        <v>0.313591269841269</v>
+      </c>
+      <c r="J22">
+        <v>0.313591269841269</v>
+      </c>
+      <c r="K22">
+        <v>0.23055555555555499</v>
+      </c>
+      <c r="L22">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="M22">
+        <v>0.31851851851851798</v>
+      </c>
+      <c r="N22">
+        <v>0.26851851851851799</v>
+      </c>
+      <c r="O22">
+        <v>0.345304232804232</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>0.33333333333333298</v>
       </c>
@@ -615,7 +927,7 @@
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>0.4</v>
       </c>
@@ -647,7 +959,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>0.66666666666666596</v>
       </c>
@@ -679,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>0.5</v>
       </c>
@@ -711,7 +1023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>0.4</v>
       </c>
@@ -743,7 +1055,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>0.6</v>
       </c>
@@ -913,15 +1225,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L36"/>
+  <dimension ref="B3:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -929,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -937,7 +1249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -945,7 +1257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -953,7 +1265,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -961,7 +1273,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -969,12 +1281,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -985,127 +1297,437 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0.1</v>
       </c>
       <c r="C13">
-        <v>0.41932350718064998</v>
+        <f>AVERAGE(F$13:F$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D13">
         <f>AVERAGE(C$27:C$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0.25</v>
+      </c>
+      <c r="G13">
+        <v>0.25</v>
+      </c>
+      <c r="H13">
+        <v>0.25</v>
+      </c>
+      <c r="I13">
+        <v>0.25</v>
+      </c>
+      <c r="J13">
+        <v>0.25</v>
+      </c>
+      <c r="K13">
+        <v>0.25</v>
+      </c>
+      <c r="L13">
+        <v>0.25</v>
+      </c>
+      <c r="M13">
+        <v>0.25</v>
+      </c>
+      <c r="N13">
+        <v>0.25</v>
+      </c>
+      <c r="O13">
+        <v>0.16666666666666599</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.2</v>
       </c>
       <c r="C14">
-        <v>0.41932350718064998</v>
+        <f>AVERAGE(G$13:G$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D14">
         <f>AVERAGE(D$27:D$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="G14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="H14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="I14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="J14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="K14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="L14">
+        <v>0.33730158730158699</v>
+      </c>
+      <c r="M14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="N14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="O14">
+        <v>0.32312925170068002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>0.3</v>
       </c>
       <c r="C15">
-        <v>0.42984930083144302</v>
+        <f>AVERAGE(H$13:H$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D15">
         <f>AVERAGE(E$27:E$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="G15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="H15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="I15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="J15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="K15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="L15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="M15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="N15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="O15">
+        <v>0.42063492063491997</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.4</v>
       </c>
       <c r="C16">
-        <v>0.41219718442932701</v>
+        <f>AVERAGE(I$13:I$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D16">
         <f>AVERAGE(F$27:F$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>0.25</v>
+      </c>
+      <c r="G16">
+        <v>0.25</v>
+      </c>
+      <c r="H16">
+        <v>0.25</v>
+      </c>
+      <c r="I16">
+        <v>0.25</v>
+      </c>
+      <c r="J16">
+        <v>0.25</v>
+      </c>
+      <c r="K16">
+        <v>0.25</v>
+      </c>
+      <c r="L16">
+        <v>0.25</v>
+      </c>
+      <c r="M16">
+        <v>0.25</v>
+      </c>
+      <c r="N16">
+        <v>0.5</v>
+      </c>
+      <c r="O16">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.5</v>
       </c>
       <c r="C17">
-        <v>0.41219718442932701</v>
+        <f>AVERAGE(J$13:J$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D17">
         <f>AVERAGE(G$27:G$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="G17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="H17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="I17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="J17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="K17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="L17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="M17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="N17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="O17">
+        <v>0.55324074074074003</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0.6</v>
       </c>
       <c r="C18">
-        <v>0.41219718442932701</v>
+        <f>AVERAGE(K$13:K$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D18">
         <f>AVERAGE(H$27:H$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="H18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="J18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="K18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="L18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="M18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="N18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="O18">
+        <v>0.49722222222222201</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0.7</v>
       </c>
       <c r="C19">
-        <v>0.402197184429327</v>
+        <f>AVERAGE(L$13:L$22)</f>
+        <v>0.46066247795414411</v>
       </c>
       <c r="D19">
         <f>AVERAGE(I$27:I$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="G19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="H19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="I19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="J19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="K19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="L19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="M19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="N19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="O19">
+        <v>0.46296296296296202</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.79999999999999905</v>
       </c>
       <c r="C20">
-        <v>0.438599300831443</v>
+        <f>AVERAGE(M$13:M$22)</f>
+        <v>0.45686429201310108</v>
       </c>
       <c r="D20">
         <f>AVERAGE(J$27:J$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="G20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="H20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="I20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="J20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="K20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="L20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="M20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="N20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="O20">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.89999999999999902</v>
       </c>
       <c r="C21">
-        <v>0.43205168178382403</v>
+        <f>AVERAGE(N$13:N$22)</f>
+        <v>0.4804919375157467</v>
       </c>
       <c r="D21">
         <f>AVERAGE(K$27:K$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="G21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="H21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="I21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="J21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="K21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="L21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="M21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="N21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="O21">
+        <v>0.54523809523809497</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.999999999999999</v>
       </c>
       <c r="C22">
-        <v>0.35987244897959098</v>
+        <f>AVERAGE(O$13:O$22)</f>
+        <v>0.37626133786848032</v>
       </c>
       <c r="D22">
         <f>AVERAGE(L$27:L$36)</f>
         <v>0.48999999999999994</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="G22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="H22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="I22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="J22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="K22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="L22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="M22">
+        <v>0.359027777777777</v>
+      </c>
+      <c r="N22">
+        <v>0.345304232804232</v>
+      </c>
+      <c r="O22">
+        <v>0.26851851851851799</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>0.33333333333333298</v>
       </c>
@@ -1137,7 +1759,7 @@
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>0.6</v>
       </c>
@@ -1169,7 +1791,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>1</v>
       </c>
@@ -1201,7 +1823,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>0.5</v>
       </c>
@@ -1233,7 +1855,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>0.4</v>
       </c>
@@ -1265,7 +1887,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>0.6</v>
       </c>
@@ -1435,15 +2057,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L120"/>
+  <dimension ref="B3:O120"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:L36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1451,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +2081,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1467,7 +2089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +2097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1483,7 +2105,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1491,12 +2113,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -1507,127 +2129,437 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13">
-        <v>0.314246031746031</v>
+        <f>AVERAGE(F$13:F$22)</f>
+        <v>0.38268783068783041</v>
       </c>
       <c r="D13">
         <f>AVERAGE(C$27:C$36)</f>
         <v>0.49666666666666648</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0.25740740740740697</v>
+      </c>
+      <c r="G13">
+        <v>0.17777777777777701</v>
+      </c>
+      <c r="H13">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="I13">
+        <v>0.25</v>
+      </c>
+      <c r="J13">
+        <v>0.36190476190476101</v>
+      </c>
+      <c r="K13">
+        <v>0.25</v>
+      </c>
+      <c r="L13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="M13">
+        <v>0.233333333333333</v>
+      </c>
+      <c r="N13">
+        <v>0.25</v>
+      </c>
+      <c r="O13">
+        <v>0.24074074074074001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>20</v>
       </c>
       <c r="C14">
-        <v>0.28587742504409103</v>
+        <f>AVERAGE(G$13:G$22)</f>
+        <v>0.41542592592592548</v>
       </c>
       <c r="D14">
         <f>AVERAGE(D$27:D$36)</f>
         <v>0.5299999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>0.238095238095238</v>
+      </c>
+      <c r="G14">
+        <v>0.19047619047618999</v>
+      </c>
+      <c r="H14">
+        <v>0.25170068027210801</v>
+      </c>
+      <c r="I14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="J14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="K14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="L14">
+        <v>0.408730158730158</v>
+      </c>
+      <c r="M14">
+        <v>0.34523809523809501</v>
+      </c>
+      <c r="N14">
+        <v>0.19999999999999901</v>
+      </c>
+      <c r="O14">
+        <v>0.25782312925169998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>30</v>
       </c>
       <c r="C15">
-        <v>0.363862433862433</v>
+        <f>AVERAGE(H$13:H$22)</f>
+        <v>0.46571151423532331</v>
       </c>
       <c r="D15">
         <f>AVERAGE(E$27:E$36)</f>
         <v>0.56999999999999984</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.407407407407407</v>
+      </c>
+      <c r="G15">
+        <v>0.59166666666666601</v>
+      </c>
+      <c r="H15">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="J15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="K15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="L15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="M15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="N15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="O15">
+        <v>0.53333333333333299</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>40</v>
       </c>
       <c r="C16">
-        <v>0.39660846560846502</v>
+        <f>AVERAGE(I$13:I$22)</f>
+        <v>0.4718325459813551</v>
       </c>
       <c r="D16">
         <f>AVERAGE(F$27:F$36)</f>
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>0.05</v>
+      </c>
+      <c r="G16">
+        <v>0.125</v>
+      </c>
+      <c r="H16">
+        <v>0.25</v>
+      </c>
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
+      </c>
+      <c r="K16">
+        <v>0.5</v>
+      </c>
+      <c r="L16">
+        <v>0.5</v>
+      </c>
+      <c r="M16">
+        <v>0.25</v>
+      </c>
+      <c r="N16">
+        <v>0.5</v>
+      </c>
+      <c r="O16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>50</v>
       </c>
       <c r="C17">
-        <v>0.38886089065255702</v>
+        <f>AVERAGE(J$13:J$22)</f>
+        <v>0.46520115268329504</v>
       </c>
       <c r="D17">
         <f>AVERAGE(G$27:G$36)</f>
         <v>0.58333333333333326</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>0.94841269841269804</v>
+      </c>
+      <c r="G17">
+        <v>0.83571428571428497</v>
+      </c>
+      <c r="H17">
+        <v>0.82182539682539602</v>
+      </c>
+      <c r="I17">
+        <v>0.43333333333333302</v>
+      </c>
+      <c r="J17">
+        <v>0.44179894179894103</v>
+      </c>
+      <c r="K17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="L17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="M17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="N17">
+        <v>0.56216931216931199</v>
+      </c>
+      <c r="O17">
+        <v>0.56216931216931199</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>60</v>
       </c>
       <c r="C18">
-        <v>0.43205168178382403</v>
+        <f>AVERAGE(K$13:K$22)</f>
+        <v>0.4804919375157467</v>
       </c>
       <c r="D18">
         <f>AVERAGE(H$27:H$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0.42</v>
+      </c>
+      <c r="G18">
+        <v>0.55333333333333301</v>
+      </c>
+      <c r="H18">
+        <v>0.61428571428571399</v>
+      </c>
+      <c r="I18">
+        <v>0.66428571428571404</v>
+      </c>
+      <c r="J18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="K18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="L18">
+        <v>0.688888888888888</v>
+      </c>
+      <c r="M18">
+        <v>0.483333333333333</v>
+      </c>
+      <c r="N18">
+        <v>0.483333333333333</v>
+      </c>
+      <c r="O18">
+        <v>0.483333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>70</v>
       </c>
       <c r="C19">
-        <v>0.48551256613756599</v>
+        <f>AVERAGE(L$13:L$22)</f>
+        <v>0.49843540564373834</v>
       </c>
       <c r="D19">
         <f>AVERAGE(I$27:I$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>0.27777777777777701</v>
+      </c>
+      <c r="G19">
+        <v>0.27777777777777701</v>
+      </c>
+      <c r="H19">
+        <v>0.36904761904761901</v>
+      </c>
+      <c r="I19">
+        <v>0.39682539682539603</v>
+      </c>
+      <c r="J19">
+        <v>0.39682539682539603</v>
+      </c>
+      <c r="K19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="L19">
+        <v>0.50617283950617198</v>
+      </c>
+      <c r="M19">
+        <v>0.50617283950617198</v>
+      </c>
+      <c r="N19">
+        <v>0.5</v>
+      </c>
+      <c r="O19">
+        <v>0.44444444444444398</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>80</v>
       </c>
       <c r="C20">
-        <v>0.46386243386243298</v>
+        <f>AVERAGE(M$13:M$22)</f>
+        <v>0.44242283950617256</v>
       </c>
       <c r="D20">
         <f>AVERAGE(J$27:J$36)</f>
         <v>0.62333333333333318</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>0.4</v>
+      </c>
+      <c r="G20">
+        <v>0.483333333333333</v>
+      </c>
+      <c r="H20">
+        <v>0.543333333333333</v>
+      </c>
+      <c r="I20">
+        <v>0.64333333333333298</v>
+      </c>
+      <c r="J20">
+        <v>0.71</v>
+      </c>
+      <c r="K20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="L20">
+        <v>0.67999999999999905</v>
+      </c>
+      <c r="M20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O20">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>90</v>
       </c>
       <c r="C21">
-        <v>0.50815003779289403</v>
+        <f>AVERAGE(N$13:N$22)</f>
+        <v>0.46317460317460296</v>
       </c>
       <c r="D21">
         <f>AVERAGE(K$27:K$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="G21">
+        <v>0.62010582010582005</v>
+      </c>
+      <c r="H21">
+        <v>0.67134038800705398</v>
+      </c>
+      <c r="I21">
+        <v>0.695414462081128</v>
+      </c>
+      <c r="J21">
+        <v>0.489682539682539</v>
+      </c>
+      <c r="K21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="L21">
+        <v>0.67949735449735404</v>
+      </c>
+      <c r="M21">
+        <v>0.76838624338624295</v>
+      </c>
+      <c r="N21">
+        <v>0.76838624338624295</v>
+      </c>
+      <c r="O21">
+        <v>0.76838624338624295</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>100</v>
       </c>
       <c r="C22">
-        <v>0.455750661375661</v>
+        <f>AVERAGE(O$13:O$22)</f>
+        <v>0.47219765684051362</v>
       </c>
       <c r="D22">
         <f>AVERAGE(L$27:L$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>0.27222222222222198</v>
+      </c>
+      <c r="G22">
+        <v>0.29907407407407399</v>
+      </c>
+      <c r="H22">
+        <v>0.31058201058201002</v>
+      </c>
+      <c r="I22">
+        <v>0.28025793650793601</v>
+      </c>
+      <c r="J22">
+        <v>0.33581349206349198</v>
+      </c>
+      <c r="K22">
+        <v>0.345304232804232</v>
+      </c>
+      <c r="L22">
+        <v>0.33263888888888798</v>
+      </c>
+      <c r="M22">
+        <v>0.34007936507936498</v>
+      </c>
+      <c r="N22">
+        <v>0.34007936507936498</v>
+      </c>
+      <c r="O22">
+        <v>0.381746031746031</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>0.33333333333333298</v>
       </c>
@@ -1659,7 +2591,7 @@
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>0.5</v>
       </c>
@@ -1691,7 +2623,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>0.33333333333333298</v>
       </c>
@@ -1723,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>0</v>
       </c>
@@ -1755,7 +2687,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>0.8</v>
       </c>
@@ -1787,7 +2719,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>0.6</v>
       </c>
@@ -1973,15 +2905,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:L36"/>
+  <dimension ref="B4:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:L36"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1989,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -1997,7 +2929,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -2005,7 +2937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -2013,7 +2945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -2021,7 +2953,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -2029,12 +2961,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -2044,128 +2976,438 @@
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0.25</v>
+      </c>
+      <c r="G13">
+        <v>0.24074074074074001</v>
+      </c>
+      <c r="H13">
+        <v>0.25</v>
+      </c>
+      <c r="I13">
+        <v>0.25</v>
+      </c>
+      <c r="J13">
+        <v>0.25</v>
+      </c>
+      <c r="K13">
+        <v>0.194444444444444</v>
+      </c>
+      <c r="L13">
+        <v>0.194444444444444</v>
+      </c>
+      <c r="M13">
+        <v>0.206349206349206</v>
+      </c>
+      <c r="N13">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="O13">
+        <v>0.17777777777777701</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.1</v>
       </c>
       <c r="C14">
-        <v>0.43205168178382403</v>
+        <f>AVERAGE(F$13:F$22)</f>
+        <v>0.4804919375157467</v>
       </c>
       <c r="D14">
         <f>AVERAGE(C$27:C$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="G14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="H14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="I14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="J14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="K14">
+        <v>0.29931972789115602</v>
+      </c>
+      <c r="L14">
+        <v>0.27551020408163202</v>
+      </c>
+      <c r="M14">
+        <v>0.27551020408163202</v>
+      </c>
+      <c r="N14">
+        <v>0.28571428571428498</v>
+      </c>
+      <c r="O14">
+        <v>0.28571428571428498</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>0.2</v>
       </c>
       <c r="C15">
-        <v>0.39620512093726301</v>
+        <f>AVERAGE(G$13:G$22)</f>
+        <v>0.45038170823885071</v>
       </c>
       <c r="D15">
         <f>AVERAGE(D$27:D$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="G15">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="H15">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="I15">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="J15">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="K15">
+        <v>0.5</v>
+      </c>
+      <c r="L15">
+        <v>0.42063492063491997</v>
+      </c>
+      <c r="M15">
+        <v>0.42063492063491997</v>
+      </c>
+      <c r="N15">
+        <v>0.42063492063491997</v>
+      </c>
+      <c r="O15">
+        <v>0.42063492063491997</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.3</v>
       </c>
       <c r="C16">
-        <v>0.37395313681027897</v>
+        <f>AVERAGE(H$13:H$22)</f>
+        <v>0.44917800453514695</v>
       </c>
       <c r="D16">
         <f>AVERAGE(E$27:E$36)</f>
         <v>0.60333333333333328</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>0.25</v>
+      </c>
+      <c r="H16">
+        <v>0.25</v>
+      </c>
+      <c r="I16">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="J16">
+        <v>0.125</v>
+      </c>
+      <c r="K16">
+        <v>0.125</v>
+      </c>
+      <c r="L16">
+        <v>0.125</v>
+      </c>
+      <c r="M16">
+        <v>0.1</v>
+      </c>
+      <c r="N16">
+        <v>0.1</v>
+      </c>
+      <c r="O16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.4</v>
       </c>
       <c r="C17">
-        <v>0.37318153187200798</v>
+        <f>AVERAGE(I$13:I$22)</f>
+        <v>0.43102985638699887</v>
       </c>
       <c r="D17">
         <f>AVERAGE(F$27:F$36)</f>
         <v>0.56333333333333324</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>0.469907407407407</v>
+      </c>
+      <c r="G17">
+        <v>0.483333333333333</v>
+      </c>
+      <c r="H17">
+        <v>0.49259259259259203</v>
+      </c>
+      <c r="I17">
+        <v>0.49259259259259203</v>
+      </c>
+      <c r="J17">
+        <v>0.504497354497354</v>
+      </c>
+      <c r="K17">
+        <v>0.504497354497354</v>
+      </c>
+      <c r="L17">
+        <v>0.504497354497354</v>
+      </c>
+      <c r="M17">
+        <v>0.411904761904761</v>
+      </c>
+      <c r="N17">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="O17">
+        <v>0.30476190476190401</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0.5</v>
       </c>
       <c r="C18">
-        <v>0.37429264298311898</v>
+        <f>AVERAGE(J$13:J$22)</f>
+        <v>0.42030234315948567</v>
       </c>
       <c r="D18">
         <f>AVERAGE(G$27:G$36)</f>
         <v>0.56333333333333324</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="G18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="H18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="J18">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="K18">
+        <v>0.65</v>
+      </c>
+      <c r="L18">
+        <v>0.65</v>
+      </c>
+      <c r="M18">
+        <v>0.688888888888888</v>
+      </c>
+      <c r="N18">
+        <v>0.688888888888888</v>
+      </c>
+      <c r="O18">
+        <v>0.688888888888888</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0.6</v>
       </c>
       <c r="C19">
-        <v>0.35864449483497102</v>
+        <f>AVERAGE(K$13:K$22)</f>
+        <v>0.40568858654572909</v>
       </c>
       <c r="D19">
         <f>AVERAGE(H$27:H$36)</f>
         <v>0.52999999999999992</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="G19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="H19">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="I19">
+        <v>0.46296296296296202</v>
+      </c>
+      <c r="J19">
+        <v>0.46296296296296202</v>
+      </c>
+      <c r="K19">
+        <v>0.42460317460317398</v>
+      </c>
+      <c r="L19">
+        <v>0.37962962962962898</v>
+      </c>
+      <c r="M19">
+        <v>0.37962962962962898</v>
+      </c>
+      <c r="N19">
+        <v>0.37962962962962898</v>
+      </c>
+      <c r="O19">
+        <v>0.344444444444444</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0.7</v>
       </c>
       <c r="C20">
-        <v>0.34863126732174299</v>
+        <f>AVERAGE(L$13:L$22)</f>
+        <v>0.39448047367094941</v>
       </c>
       <c r="D20">
         <f>AVERAGE(I$27:I$36)</f>
         <v>0.4966666666666667</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="G20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="H20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="I20">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="J20">
+        <v>0.65</v>
+      </c>
+      <c r="K20">
+        <v>0.62</v>
+      </c>
+      <c r="L20">
+        <v>0.60888888888888804</v>
+      </c>
+      <c r="M20">
+        <v>0.45333333333333298</v>
+      </c>
+      <c r="N20">
+        <v>0.45333333333333298</v>
+      </c>
+      <c r="O20">
+        <v>0.353333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0.79999999999999905</v>
       </c>
       <c r="C21">
-        <v>0.337681531872008</v>
+        <f>AVERAGE(M$13:M$22)</f>
+        <v>0.3716277399848823</v>
       </c>
       <c r="D21">
         <f>AVERAGE(J$27:J$36)</f>
         <v>0.4966666666666667</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>0.63165784832451399</v>
+      </c>
+      <c r="G21">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="H21">
+        <v>0.51666666666666605</v>
+      </c>
+      <c r="I21">
+        <v>0.44999999999999901</v>
+      </c>
+      <c r="J21">
+        <v>0.43677248677248598</v>
+      </c>
+      <c r="K21">
+        <v>0.43677248677248598</v>
+      </c>
+      <c r="L21">
+        <v>0.48395061728395</v>
+      </c>
+      <c r="M21">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="N21">
+        <v>0.47777777777777702</v>
+      </c>
+      <c r="O21">
+        <v>0.44999999999999901</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0.89999999999999902</v>
       </c>
       <c r="C22">
-        <v>0.31822121441168999</v>
+        <f>AVERAGE(N$13:N$22)</f>
+        <v>0.37304497354497307</v>
       </c>
       <c r="D22">
         <f>AVERAGE(K$27:K$36)</f>
         <v>0.4966666666666667</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>0.345304232804232</v>
+      </c>
+      <c r="G22">
+        <v>0.33280423280423199</v>
+      </c>
+      <c r="H22">
+        <v>0.31891534391534299</v>
+      </c>
+      <c r="I22">
+        <v>0.30224867724867699</v>
+      </c>
+      <c r="J22">
+        <v>0.30224867724867699</v>
+      </c>
+      <c r="K22">
+        <v>0.30224867724867699</v>
+      </c>
+      <c r="L22">
+        <v>0.30224867724867699</v>
+      </c>
+      <c r="M22">
+        <v>0.30224867724867699</v>
+      </c>
+      <c r="N22">
+        <v>0.30224867724867699</v>
+      </c>
+      <c r="O22">
+        <v>0.30224867724867699</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0.999999999999999</v>
       </c>
       <c r="C23">
-        <v>0.30054661123708698</v>
+        <f>AVERAGE(O$13:O$22)</f>
+        <v>0.34278042328042269</v>
       </c>
       <c r="D23">
         <f>AVERAGE(L$27:L$36)</f>
         <v>0.4966666666666667</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>0.33333333333333298</v>
       </c>
@@ -2197,7 +3439,7 @@
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>0.4</v>
       </c>
@@ -2229,7 +3471,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>1</v>
       </c>
@@ -2261,7 +3503,7 @@
         <v>0.33333333333333298</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>0.5</v>
       </c>
@@ -2293,7 +3535,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>0.4</v>
       </c>
@@ -2325,7 +3567,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C32">
         <v>0.6</v>
       </c>
@@ -2498,7 +3740,7 @@
   <dimension ref="B4:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C14" sqref="C14:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Yahoo index and a couple more graphs added
</commit_message>
<xml_diff>
--- a/Results/OkapiBM-25.xlsx
+++ b/Results/OkapiBM-25.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="alpha" sheetId="1" r:id="rId1"/>
     <sheet name="beta" sheetId="2" r:id="rId2"/>
     <sheet name="terms" sheetId="4" r:id="rId3"/>
-    <sheet name="b" sheetId="5" r:id="rId4"/>
-    <sheet name="bm25_k" sheetId="6" r:id="rId5"/>
-    <sheet name="k" sheetId="7" r:id="rId6"/>
+    <sheet name="modified-okp" sheetId="8" r:id="rId4"/>
+    <sheet name="okp vs modified okp" sheetId="9" r:id="rId5"/>
+    <sheet name="b" sheetId="5" r:id="rId6"/>
+    <sheet name="bm25_k" sheetId="6" r:id="rId7"/>
+    <sheet name="k" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="11">
   <si>
     <t>Beta</t>
   </si>
@@ -2059,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:O22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2904,6 +2906,963 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:P36"/>
+  <sheetViews>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>0.25740740740740697</v>
+      </c>
+      <c r="H13">
+        <v>0.25740740740740697</v>
+      </c>
+      <c r="I13">
+        <v>0.28518518518518499</v>
+      </c>
+      <c r="J13">
+        <v>0.25740740740740697</v>
+      </c>
+      <c r="K13">
+        <v>0.28518518518518499</v>
+      </c>
+      <c r="L13">
+        <v>0.28518518518518499</v>
+      </c>
+      <c r="M13">
+        <v>0.28518518518518499</v>
+      </c>
+      <c r="N13">
+        <v>0.28518518518518499</v>
+      </c>
+      <c r="O13">
+        <v>0.34074074074074001</v>
+      </c>
+      <c r="P13">
+        <v>0.34074074074074001</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE(G$13:G$22)</f>
+        <v>0.38507652246990459</v>
+      </c>
+      <c r="E14">
+        <f>AVERAGE(D$27:D$36)</f>
+        <v>0.47666666666666668</v>
+      </c>
+      <c r="G14">
+        <v>0.238095238095238</v>
+      </c>
+      <c r="H14">
+        <v>0.238095238095238</v>
+      </c>
+      <c r="I14">
+        <v>0.26785714285714202</v>
+      </c>
+      <c r="J14">
+        <v>0.331349206349206</v>
+      </c>
+      <c r="K14">
+        <v>0.331349206349206</v>
+      </c>
+      <c r="L14">
+        <v>0.331349206349206</v>
+      </c>
+      <c r="M14">
+        <v>0.331349206349206</v>
+      </c>
+      <c r="N14">
+        <v>0.331349206349206</v>
+      </c>
+      <c r="O14">
+        <v>0.31706349206349199</v>
+      </c>
+      <c r="P14">
+        <v>0.44563492063492</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(H$13:H$22)</f>
+        <v>0.45254676804676769</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(E$27:E$36)</f>
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="G15">
+        <v>0.407407407407407</v>
+      </c>
+      <c r="H15">
+        <v>0.51190476190476097</v>
+      </c>
+      <c r="I15">
+        <v>0.52777777777777701</v>
+      </c>
+      <c r="J15">
+        <v>0.56666666666666599</v>
+      </c>
+      <c r="K15">
+        <v>0.56666666666666599</v>
+      </c>
+      <c r="L15">
+        <v>0.59166666666666601</v>
+      </c>
+      <c r="M15">
+        <v>0.60952380952380902</v>
+      </c>
+      <c r="N15">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="O15">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="P15">
+        <v>0.63333333333333297</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(I$13:I$22)</f>
+        <v>0.50429863752232129</v>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(F$27:F$36)</f>
+        <v>0.48666666666666653</v>
+      </c>
+      <c r="G16">
+        <v>0.05</v>
+      </c>
+      <c r="H16">
+        <v>0.1</v>
+      </c>
+      <c r="I16">
+        <v>0.15</v>
+      </c>
+      <c r="J16">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="L16">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="M16">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="N16">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="O16">
+        <v>0.1875</v>
+      </c>
+      <c r="P16">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <f>AVERAGE(J$13:J$22)</f>
+        <v>0.50953726597476556</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(G$27:G$36)</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G17">
+        <v>0.94841269841269804</v>
+      </c>
+      <c r="H17">
+        <v>0.94841269841269804</v>
+      </c>
+      <c r="I17">
+        <v>0.94841269841269804</v>
+      </c>
+      <c r="J17">
+        <v>0.87738095238095204</v>
+      </c>
+      <c r="K17">
+        <v>0.97619047619047605</v>
+      </c>
+      <c r="L17">
+        <v>0.93055555555555503</v>
+      </c>
+      <c r="M17">
+        <v>0.93055555555555503</v>
+      </c>
+      <c r="N17">
+        <v>0.93055555555555503</v>
+      </c>
+      <c r="O17">
+        <v>0.97619047619047605</v>
+      </c>
+      <c r="P17">
+        <v>0.97619047619047605</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <f>AVERAGE(K$13:K$22)</f>
+        <v>0.52108132376882343</v>
+      </c>
+      <c r="E18">
+        <f>AVERAGE(H$27:H$36)</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="G18">
+        <v>0.42</v>
+      </c>
+      <c r="H18">
+        <v>0.55333333333333301</v>
+      </c>
+      <c r="I18">
+        <v>0.65333333333333299</v>
+      </c>
+      <c r="J18">
+        <v>0.65333333333333299</v>
+      </c>
+      <c r="K18">
+        <v>0.65333333333333299</v>
+      </c>
+      <c r="L18">
+        <v>0.65333333333333299</v>
+      </c>
+      <c r="M18">
+        <v>0.65333333333333299</v>
+      </c>
+      <c r="N18">
+        <v>0.72</v>
+      </c>
+      <c r="O18">
+        <v>0.72</v>
+      </c>
+      <c r="P18">
+        <v>0.71583333333333299</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <f>AVERAGE(L$13:L$22)</f>
+        <v>0.53313696420681678</v>
+      </c>
+      <c r="E19">
+        <f>AVERAGE(I$27:I$36)</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="G19">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H19">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="I19">
+        <v>0.38888888888888801</v>
+      </c>
+      <c r="J19">
+        <v>0.38888888888888801</v>
+      </c>
+      <c r="K19">
+        <v>0.38888888888888801</v>
+      </c>
+      <c r="L19">
+        <v>0.51298701298701199</v>
+      </c>
+      <c r="M19">
+        <v>0.562715062715062</v>
+      </c>
+      <c r="N19">
+        <v>0.57329707329707302</v>
+      </c>
+      <c r="O19">
+        <v>0.56054131054130996</v>
+      </c>
+      <c r="P19">
+        <v>0.54961334961334896</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>70</v>
+      </c>
+      <c r="D20">
+        <f>AVERAGE(M$13:M$22)</f>
+        <v>0.54122799787931331</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGE(J$27:J$36)</f>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="G20">
+        <v>0.3</v>
+      </c>
+      <c r="H20">
+        <v>0.53939393939393898</v>
+      </c>
+      <c r="I20">
+        <v>0.65142857142857102</v>
+      </c>
+      <c r="J20">
+        <v>0.67678571428571399</v>
+      </c>
+      <c r="K20">
+        <v>0.66428571428571404</v>
+      </c>
+      <c r="L20">
+        <v>0.661904761904761</v>
+      </c>
+      <c r="M20">
+        <v>0.65974025974025896</v>
+      </c>
+      <c r="N20">
+        <v>0.65776397515527896</v>
+      </c>
+      <c r="O20">
+        <v>0.65776397515527896</v>
+      </c>
+      <c r="P20">
+        <v>0.65776397515527896</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>80</v>
+      </c>
+      <c r="D21">
+        <f>AVERAGE(N$13:N$22)</f>
+        <v>0.55847750904954985</v>
+      </c>
+      <c r="E21">
+        <f>AVERAGE(K$27:K$36)</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G21">
+        <v>0.57043512043512001</v>
+      </c>
+      <c r="H21">
+        <v>0.60170940170940101</v>
+      </c>
+      <c r="I21">
+        <v>0.66420940170940101</v>
+      </c>
+      <c r="J21">
+        <v>0.65991045991046005</v>
+      </c>
+      <c r="K21">
+        <v>0.65805860805860805</v>
+      </c>
+      <c r="L21">
+        <v>0.65805860805860805</v>
+      </c>
+      <c r="M21">
+        <v>0.67974987974987899</v>
+      </c>
+      <c r="N21">
+        <v>0.70646945646945603</v>
+      </c>
+      <c r="O21">
+        <v>0.70646945646945603</v>
+      </c>
+      <c r="P21">
+        <v>0.70646945646945603</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <f>AVERAGE(O$13:O$22)</f>
+        <v>0.56839240896444976</v>
+      </c>
+      <c r="E22">
+        <f>AVERAGE(L$27:L$36)</f>
+        <v>0.58999999999999986</v>
+      </c>
+      <c r="G22">
+        <v>0.32567401960784298</v>
+      </c>
+      <c r="H22">
+        <v>0.44187756687756602</v>
+      </c>
+      <c r="I22">
+        <v>0.50589337563021697</v>
+      </c>
+      <c r="J22">
+        <v>0.52115003052502995</v>
+      </c>
+      <c r="K22">
+        <v>0.52435515873015803</v>
+      </c>
+      <c r="L22">
+        <v>0.54382931202784102</v>
+      </c>
+      <c r="M22">
+        <v>0.53762768664084404</v>
+      </c>
+      <c r="N22">
+        <v>0.58432130515041203</v>
+      </c>
+      <c r="O22">
+        <v>0.58432130515041203</v>
+      </c>
+      <c r="P22">
+        <v>0.58432130515041203</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE(P$13:P$22)</f>
+        <v>0.5797400890621297</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(M$27:M$36)</f>
+        <v>0.58999999999999986</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="H27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="I27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="L27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M27">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0.5</v>
+      </c>
+      <c r="E28">
+        <v>0.4</v>
+      </c>
+      <c r="F28">
+        <v>0.4</v>
+      </c>
+      <c r="G28">
+        <v>0.4</v>
+      </c>
+      <c r="H28">
+        <v>0.4</v>
+      </c>
+      <c r="I28">
+        <v>0.4</v>
+      </c>
+      <c r="J28">
+        <v>0.4</v>
+      </c>
+      <c r="K28">
+        <v>0.4</v>
+      </c>
+      <c r="L28">
+        <v>0.4</v>
+      </c>
+      <c r="M28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="E29">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F29">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G29">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="H29">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="I29">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="J29">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="K29">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="L29">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="M29">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0.5</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0.5</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+      <c r="I30">
+        <v>0.5</v>
+      </c>
+      <c r="J30">
+        <v>0.5</v>
+      </c>
+      <c r="K30">
+        <v>0.5</v>
+      </c>
+      <c r="L30">
+        <v>0.5</v>
+      </c>
+      <c r="M30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>0.8</v>
+      </c>
+      <c r="E31">
+        <v>0.8</v>
+      </c>
+      <c r="F31">
+        <v>0.8</v>
+      </c>
+      <c r="G31">
+        <v>0.8</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0.8</v>
+      </c>
+      <c r="J31">
+        <v>0.8</v>
+      </c>
+      <c r="K31">
+        <v>0.8</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>0.6</v>
+      </c>
+      <c r="E32">
+        <v>0.6</v>
+      </c>
+      <c r="F32">
+        <v>0.6</v>
+      </c>
+      <c r="G32">
+        <v>0.6</v>
+      </c>
+      <c r="H32">
+        <v>0.6</v>
+      </c>
+      <c r="I32">
+        <v>0.6</v>
+      </c>
+      <c r="J32">
+        <v>0.6</v>
+      </c>
+      <c r="K32">
+        <v>0.6</v>
+      </c>
+      <c r="L32">
+        <v>0.6</v>
+      </c>
+      <c r="M32">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>0.6</v>
+      </c>
+      <c r="E33">
+        <v>0.6</v>
+      </c>
+      <c r="F33">
+        <v>0.6</v>
+      </c>
+      <c r="G33">
+        <v>0.6</v>
+      </c>
+      <c r="H33">
+        <v>0.6</v>
+      </c>
+      <c r="I33">
+        <v>0.6</v>
+      </c>
+      <c r="J33">
+        <v>0.6</v>
+      </c>
+      <c r="K33">
+        <v>0.6</v>
+      </c>
+      <c r="L33">
+        <v>0.6</v>
+      </c>
+      <c r="M33">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>0.4</v>
+      </c>
+      <c r="E34">
+        <v>0.4</v>
+      </c>
+      <c r="F34">
+        <v>0.4</v>
+      </c>
+      <c r="G34">
+        <v>0.4</v>
+      </c>
+      <c r="H34">
+        <v>0.4</v>
+      </c>
+      <c r="I34">
+        <v>0.4</v>
+      </c>
+      <c r="J34">
+        <v>0.4</v>
+      </c>
+      <c r="K34">
+        <v>0.4</v>
+      </c>
+      <c r="L34">
+        <v>0.4</v>
+      </c>
+      <c r="M34">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>0.8</v>
+      </c>
+      <c r="E35">
+        <v>0.8</v>
+      </c>
+      <c r="F35">
+        <v>0.8</v>
+      </c>
+      <c r="G35">
+        <v>0.8</v>
+      </c>
+      <c r="H35">
+        <v>0.6</v>
+      </c>
+      <c r="I35">
+        <v>0.6</v>
+      </c>
+      <c r="J35">
+        <v>0.6</v>
+      </c>
+      <c r="K35">
+        <v>0.8</v>
+      </c>
+      <c r="L35">
+        <v>0.8</v>
+      </c>
+      <c r="M35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>0.4</v>
+      </c>
+      <c r="E36">
+        <v>0.4</v>
+      </c>
+      <c r="F36">
+        <v>0.6</v>
+      </c>
+      <c r="G36">
+        <v>0.4</v>
+      </c>
+      <c r="H36">
+        <v>0.4</v>
+      </c>
+      <c r="I36">
+        <v>0.6</v>
+      </c>
+      <c r="J36">
+        <v>0.6</v>
+      </c>
+      <c r="K36">
+        <v>0.6</v>
+      </c>
+      <c r="L36">
+        <v>0.6</v>
+      </c>
+      <c r="M36">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B6:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.49666666666666648</v>
+      </c>
+      <c r="D6">
+        <v>0.47666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>0.5299999999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.51666666666666672</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>0.56999999999999984</v>
+      </c>
+      <c r="D8">
+        <v>0.48666666666666653</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D9">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="D10">
+        <v>0.54999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>0.60333333333333328</v>
+      </c>
+      <c r="D11">
+        <v>0.54999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>0.62333333333333318</v>
+      </c>
+      <c r="D12">
+        <v>0.54999999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>0.62333333333333318</v>
+      </c>
+      <c r="D13">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>90</v>
+      </c>
+      <c r="C14">
+        <v>0.60333333333333328</v>
+      </c>
+      <c r="D14">
+        <v>0.58999999999999986</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>0.60333333333333328</v>
+      </c>
+      <c r="D15">
+        <v>0.58999999999999986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:O36"/>
   <sheetViews>
@@ -3735,7 +4694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D22"/>
   <sheetViews>
@@ -3916,7 +4875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D23"/>
   <sheetViews>

</xml_diff>

<commit_message>
Graphs for Yahoo added
</commit_message>
<xml_diff>
--- a/Results/OkapiBM-25.xlsx
+++ b/Results/OkapiBM-25.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="alpha" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,11 @@
     <sheet name="terms" sheetId="4" r:id="rId3"/>
     <sheet name="modified-okp" sheetId="8" r:id="rId4"/>
     <sheet name="okp vs modified okp" sheetId="9" r:id="rId5"/>
-    <sheet name="b" sheetId="5" r:id="rId6"/>
-    <sheet name="bm25_k" sheetId="6" r:id="rId7"/>
-    <sheet name="k" sheetId="7" r:id="rId8"/>
+    <sheet name="Yahoo" sheetId="10" r:id="rId6"/>
+    <sheet name="Yahoo-P5" sheetId="11" r:id="rId7"/>
+    <sheet name="b" sheetId="5" r:id="rId8"/>
+    <sheet name="bm25_k" sheetId="6" r:id="rId9"/>
+    <sheet name="k" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="13">
   <si>
     <t>Beta</t>
   </si>
@@ -64,6 +66,12 @@
   </si>
   <si>
     <t>param</t>
+  </si>
+  <si>
+    <t>Okapi</t>
+  </si>
+  <si>
+    <t>Modified</t>
   </si>
 </sst>
 </file>
@@ -1225,6 +1233,198 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D14">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D15">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D16">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D17">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D18">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D19">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D20">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D21">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>90</v>
+      </c>
+      <c r="C22">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D22">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>0.43205168178382403</v>
+      </c>
+      <c r="D23">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O36"/>
@@ -2061,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O120"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D22"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3741,7 +3941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:D15"/>
     </sheetView>
   </sheetViews>
@@ -3863,6 +4063,541 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0.32677326486149999</v>
+      </c>
+      <c r="D12">
+        <v>0.363888158016556</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>0.28547018349639502</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>0.40415466257424898</v>
+      </c>
+      <c r="D13">
+        <v>0.48503560279667302</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>0.25797053345035198</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>0.41059320181973402</v>
+      </c>
+      <c r="D14">
+        <v>0.53584558817493</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>0.29507013997824499</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>0.42503030822257898</v>
+      </c>
+      <c r="D15">
+        <v>0.56249436120117802</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="I15">
+        <v>0.29708722334079102</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>0.41685507181595999</v>
+      </c>
+      <c r="D16">
+        <v>0.57596057032997505</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>0.300780119589449</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>0.40551061470687499</v>
+      </c>
+      <c r="D17">
+        <v>0.57664356364448499</v>
+      </c>
+      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>0.30135146774284499</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>70</v>
+      </c>
+      <c r="C18">
+        <v>0.40147692676361302</v>
+      </c>
+      <c r="D18">
+        <v>0.58038825491416102</v>
+      </c>
+      <c r="G18">
+        <v>70</v>
+      </c>
+      <c r="I18">
+        <v>0.29518761625474998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>0.412084301805828</v>
+      </c>
+      <c r="D19">
+        <v>0.59634404038995104</v>
+      </c>
+      <c r="G19">
+        <v>80</v>
+      </c>
+      <c r="I19">
+        <v>0.29824675026832598</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <v>0.44792270099529102</v>
+      </c>
+      <c r="D20">
+        <v>0.60604020628258604</v>
+      </c>
+      <c r="G20">
+        <v>90</v>
+      </c>
+      <c r="I20">
+        <v>0.29455371527955299</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>0.46024212433200201</v>
+      </c>
+      <c r="D21">
+        <v>0.60792912358442797</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="I21">
+        <v>0.29279047230073202</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" display="P@K"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0.6</v>
+      </c>
+      <c r="D13">
+        <v>0.6</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>0.6</v>
+      </c>
+      <c r="I13">
+        <v>0.38873012632302001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>0.72</v>
+      </c>
+      <c r="D14">
+        <v>0.7</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>0.7</v>
+      </c>
+      <c r="I14">
+        <v>0.32998316455372201</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>0.74</v>
+      </c>
+      <c r="D15">
+        <v>0.74</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>0.74</v>
+      </c>
+      <c r="I15">
+        <v>0.327278338896895</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16">
+        <v>0.74</v>
+      </c>
+      <c r="D16">
+        <v>0.74</v>
+      </c>
+      <c r="G16">
+        <v>40</v>
+      </c>
+      <c r="H16">
+        <v>0.74</v>
+      </c>
+      <c r="I16">
+        <v>0.327278338896895</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>0.67999999999999905</v>
+      </c>
+      <c r="D17">
+        <v>0.74</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>0.74</v>
+      </c>
+      <c r="I17">
+        <v>0.34058772731852799</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>0.7</v>
+      </c>
+      <c r="D18">
+        <v>0.74</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="H18">
+        <v>0.74</v>
+      </c>
+      <c r="I18">
+        <v>0.34058772731852799</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>70</v>
+      </c>
+      <c r="C19">
+        <v>0.72</v>
+      </c>
+      <c r="D19">
+        <v>0.74</v>
+      </c>
+      <c r="G19">
+        <v>70</v>
+      </c>
+      <c r="H19">
+        <v>0.74</v>
+      </c>
+      <c r="I19">
+        <v>0.34058772731852799</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>80</v>
+      </c>
+      <c r="C20">
+        <v>0.74</v>
+      </c>
+      <c r="D20">
+        <v>0.74</v>
+      </c>
+      <c r="G20">
+        <v>80</v>
+      </c>
+      <c r="H20">
+        <v>0.74</v>
+      </c>
+      <c r="I20">
+        <v>0.34058772731852799</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>90</v>
+      </c>
+      <c r="C21">
+        <v>0.74</v>
+      </c>
+      <c r="D21">
+        <v>0.74</v>
+      </c>
+      <c r="G21">
+        <v>90</v>
+      </c>
+      <c r="H21">
+        <v>0.74</v>
+      </c>
+      <c r="I21">
+        <v>0.35339622081862798</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>0.74</v>
+      </c>
+      <c r="D22">
+        <v>0.74</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>0.74</v>
+      </c>
+      <c r="I22">
+        <v>0.35339622081862798</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1" display="P@K"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:O36"/>
   <sheetViews>
@@ -4694,7 +5429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D22"/>
   <sheetViews>
@@ -4873,196 +5608,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D14">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D15">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>30</v>
-      </c>
-      <c r="C16">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D16">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>40</v>
-      </c>
-      <c r="C17">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D17">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D18">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>60</v>
-      </c>
-      <c r="C19">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D19">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>70</v>
-      </c>
-      <c r="C20">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D20">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>80</v>
-      </c>
-      <c r="C21">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D21">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>90</v>
-      </c>
-      <c r="C22">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D22">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>100</v>
-      </c>
-      <c r="C23">
-        <v>0.43205168178382403</v>
-      </c>
-      <c r="D23">
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>